<commit_message>
tự động gửi mail theo cấu hình
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/excel-templates/Cell2G_Inventory_Rims.xlsx
+++ b/src/main/webapp/WEB-INF/excel-templates/Cell2G_Inventory_Rims.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6EF92745-A798-4612-9280-A115310CBD25}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{76A21D16-2E85-410E-8160-702481EF46A9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>CELL_NAME</t>
   </si>
@@ -34,18 +34,6 @@
     <t>FREQUENCY_BAND</t>
   </si>
   <si>
-    <t>BCCH</t>
-  </si>
-  <si>
-    <t>BSIC</t>
-  </si>
-  <si>
-    <t>TCH</t>
-  </si>
-  <si>
-    <t>TRX_CONFIG</t>
-  </si>
-  <si>
     <t>BSC_RNC_NAME</t>
   </si>
   <si>
@@ -55,9 +43,6 @@
     <t>VENDOR</t>
   </si>
   <si>
-    <t>FILENAME</t>
-  </si>
-  <si>
     <t>CHECK_DATE</t>
   </si>
   <si>
@@ -65,6 +50,12 @@
   </si>
   <si>
     <t>Danh sách cell 2G trên Inventory không có trên RIMS</t>
+  </si>
+  <si>
+    <t>TỈNH/TP</t>
+  </si>
+  <si>
+    <t>KHU VỰC</t>
   </si>
 </sst>
 </file>
@@ -80,6 +71,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
@@ -129,8 +121,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,59 +415,51 @@
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
-    <col min="12" max="13" width="12.28515625" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>